<commit_message>
add card links to clips
</commit_message>
<xml_diff>
--- a/videos.xlsx
+++ b/videos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="493">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -39,6 +39,21 @@
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExerciseLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShortLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YoutubeLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links</t>
   </si>
   <si>
     <t xml:space="preserve">Helyiérték-táblázat</t>
@@ -59,6 +74,25 @@
 07:40:23</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LsUmDFy3jZPYoZ0X9zU
+https://zsebtanar.hu/exercise/-LsUp6V5QinYBhDXkgHq
+https://zsebtanar.hu/exercise/-LsUpmr2uSpWYeJSzIsQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/334pYHg
+http://bit.ly/2Qz734H
+http://bit.ly/2O2CT8l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/gJ4XDBpLRv4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helyiérték táblázat,helyiértékes szöveges feladatok,matematika 5. osztály,szöveges feladatok 5. osztály,helyiérték-táblázat,helyiérték táblázat feladatok,helyiérték táblázat 5 osztály,helyi érték jelentése,helyi érték gyakorlása,helyi érték táblázat,helyi érték fogalma,helyi érték tanítása,helyi érték,matematika 5. osztály tananyag,matematika,5. osztály,5. osztály matematika,5. osztály matematika tananyag,5. osztály matematika feladatok,5. osztály matek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:44 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alaki érték, helyiérték, valódi érték</t>
   </si>
   <si>
@@ -77,6 +111,25 @@
 03:58:19</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LsUv9SdszTF925x3yuf
+https://zsebtanar.hu/exercise/-LsUvbR8wcxN312Owoj9
+https://zsebtanar.hu/exercise/-LsUvzUP6MkuSziUxvP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/35vikHE
+http://bit.ly/2qtMFHJ
+http://bit.ly/2quql0C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/zmXwLgaKu_w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alaki érték fogalma,alaki érték helyi érték valódi érték,alaki érték helyi érték,alaki érték jelentése,alaki érték példa,alaki érték valódi érték,alaki értékű szám,helyi érték alaki érték valódi érték,helyi érték valódi érték alaki érték,helyi érték valódi érték,helyiérték alaki érték valódi érték,helyiérték valódi érték,valódi érték alaki érték,valódi érték feladatok,valódi érték fogalma,valódi érték helyi érték,helyiérték,alaki érték,valódi érték</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:36 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Római számok</t>
   </si>
   <si>
@@ -90,6 +143,23 @@
   <si>
     <t xml:space="preserve">04:34:18
 09:38:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LsizCR5ForAziAMPkim
+https://zsebtanar.hu/exercise/-Lsj-aLXb9x63LViuJNa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2DaTxMK
+http://bit.ly/33a6Fw5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/7RXCFMV0wAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">római számok, római számok bevezetése, római számok youtube, római számok gyakorlása, római számok írása, római számok szabálya, a római számok írásának szabályai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:35 - 000</t>
   </si>
   <si>
     <t xml:space="preserve">Számegyenes</t>
@@ -113,6 +183,27 @@
 07:29:07</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LsjSvwdDpZRTByXgigM
+https://zsebtanar.hu/exercise/-LsjWzpJ2jvTnyo6bkdz
+https://zsebtanar.hu/exercise/-LsjZZjjjQOiQJfE3eVx
+https://zsebtanar.hu/exercise/-LsjaBleDf27DGS3LbVJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2OiuHAJ
+http://bit.ly/2Oiv0LT
+http://bit.ly/2OIYtxH
+http://bit.ly/2QQ9gbX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/ujxtI0BxSHc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">számegyenesek intervallumok,számegyenesen való ábrázolás,számegyenes 5. osztály,számegyenes intervallum,számegyenes jelölések,számegyenesek,számegyenes egyenlőtlenség,számegyenes intervallum feladatok,számegyenes feladatok,számegyenes ábrázolás,számegyenesen jelölés,számegyenes,szám egyenes,szám egyenes feladatok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:35 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Írásbeli összeadás</t>
   </si>
   <si>
@@ -131,6 +222,25 @@
 07:40:16</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-Lu_wGvCIFP-_kZ_poBE
+https://zsebtanar.hu/exercise/-Lu_xNpvyP_S1y0GjV-7
+https://zsebtanar.hu/exercise/-Lu_xmCajMMTtdXaMyz-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2OJbUxM
+http://bit.ly/33mi8IY
+http://bit.ly/34jUTAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/CEV8ZObbISQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">összeadás kivonás,összeadások,összeadás kivonás szabályai,összeadás bevezetése,összeadás feladatok,összeadás gyakorlása 5. osztály,írásbeli összeadás,összeadás kivonás írásban,összeadás kivonás egész számokkal,összeadás kivonás háromjegyű számokkal,összeadás papíron,írásbeli összeadás,írásbeli összeadás tanítása,írásbeli összeadás tanítása 5. osztály,írásbeli összeadás 5. osztály,egész számok összeadása kivonása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:36 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Írásbeli kivonás</t>
   </si>
   <si>
@@ -144,6 +254,23 @@
   <si>
     <t xml:space="preserve">03:23:29
 06:00:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-Luf3xKxs4e1MUrCHWal
+https://zsebtanar.hu/exercise/-Luf8hkkAhWhf0GqKN0O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2DqvPMp
+http://bit.ly/2pYld4w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/SyV3JunrSyk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kivonás gyakorlása,kivonás papíron,a kivonás szabályai,a kivonás tagjai,kivonás gyakorlása 5. osztály,kivonás írásban,matematika kivonás,összeadás kivonás,összeadás kivonás szabályai,kivonás szabályai,kivonás 100-as számkörben,természetes számok kivonása,számok kivonása,egész számok kivonása,írásbeli kivonás 5. osztály feladatok,írásbeli kivonás gyakorlása,írásbeli kivonás pótlással,írásbeli kivonás szabályai,írásbeli kivonás menete,írásbeli kivonás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:24 - 000</t>
   </si>
   <si>
     <t xml:space="preserve">Egész számok szorzása írásban</t>
@@ -164,6 +291,25 @@
 10:32:14</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LvYMj11OAspVh2Dhk3W
+https://zsebtanar.hu/exercise/-LvYNtBYuZ4e_rsZkxtW
+https://zsebtanar.hu/exercise/-LvYOPW9MxKs3pBCfwwC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2DVgm7t
+http://bit.ly/352olLQ
+http://bit.ly/38dXYVk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/3oXhHIUH4ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">szorzás 5. osztály,szorzas egész szamokkal,szorzas osztas gyakorlatok,szorzás írásban,szorzas osztas irasban,szorzás kétjegyűvel,szorzás levezetése,szorzas osztas papiron,szorzas ketjegyu szamokkal,osztas szorzas gyakorlatok,szorzás papíron,szorzás egyszerűen,szorzás egyjegyűvel,írásbeli szorzás egyjegyű szorzóval,írásbeli szorzás 5.osztály,írásbeli szorzás feladatlap,egész számok szorzása egész számmal,egész számok szorzása osztása,írásbeli szorzás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:50 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Írásbeli osztás</t>
   </si>
   <si>
@@ -177,6 +323,23 @@
   <si>
     <t xml:space="preserve">06:13:14
 08:04:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LvZ8Mtw_tcnKGKZZAeO
+https://zsebtanar.hu/exercise/-Lvi6X3PrNuoWmytZsjI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/36jEdK7
+http://bit.ly/2PubRGn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/UIsxl8Ou7QU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">írásbeli osztás 5. osztály,írásbeli osztás többjegyű osztóval,írásbeli osztás egyjegyűvel,írásbeli osztás gyakorlása,írásbeli osztás gyakorlása 4. osztály,írásbeli osztás kétjegyű osztóval,írásbeli osztás példa,írásbeli osztás szabályai,írásbeli osztás 1 jegyű osztóval,osztás egész számokkal,maradékos osztás 5. osztály,maradékos osztás kétjegyűvel,egész számok osztása,írásbeli osztás,maradékos osztás,bennfoglalás 5. osztály,bennfoglalás osztás</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:13 - 000</t>
   </si>
   <si>
     <t xml:space="preserve">Kerekítés, becslés</t>
@@ -195,6 +358,25 @@
     <t xml:space="preserve">03:14:00
 06:10:13
 07:54:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LwH5rj4Azxx0a95D3LX
+https://zsebtanar.hu/exercise/-LwH8HWUGwizj73inPbO
+https://zsebtanar.hu/exercise/-LwHGxtLyP76NVPhbuWC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2M1iKhu
+http://bit.ly/2PquTi6
+http://bit.ly/2sxgtUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/t-T4ccWTJlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">becslés 5. osztály,becslés kerekítés,becslés lényege 5. osztály,becslés feladatok,becslés feladatok megoldással,becslés lényege,becslés gyakorlása,becslés matematika 5. osztály,kerekítés szabályai,kerekítés feladatok 5 osztály,kerekítés tízesre,kerekítés százasra,a kerekítés matematikai szabályai,kerekítés ezresekre,kerekítés matematikai szabályai,kerekítés 5. osztály,kerekítés 1000-re,kerekítés 10-re,kerekítés,becslés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:14 - 000</t>
   </si>
   <si>
     <t xml:space="preserve">Osztó, többszörös</t>
@@ -218,6 +400,27 @@
 13:58:12</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LwHSzNHm74aKpSjw_CP
+https://zsebtanar.hu/exercise/-LwHTny1klpgmeNbHStV
+https://zsebtanar.hu/exercise/-LwHUkRF8n0X1L11cH1v
+https://zsebtanar.hu/exercise/-LwHVVMWw1kvIdae6yhY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/35tgvLJ
+http://bit.ly/35uiZJI
+http://bit.ly/2LYLp6M
+http://bit.ly/2PRUmzZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/CkxLOWE_IYI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">osztó többszörös,osztók száma,osztópárok,osztó fogalma,számok osztói,egy szám osztóinak megkeresése,osztó kiszámítása,osztó többszörös fogalma,közös osztó kiszámítása,közös osztók száma,közös osztó fogalma,közös osztó meghatározása,oszthatósági szabályok 5. osztály,oszthatóság 6. osztály,oszthatósági feladatok,oszthatósági feladatok 6. osztály,oszthatóság feladatok,oszthatóság szabályai,oszthatóság tulajdonságai,oszthatóság 4-gyel,oszthatóság 5 osztály</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:47 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kettes számrendszer</t>
   </si>
   <si>
@@ -242,6 +445,27 @@
     <t xml:space="preserve">kód beírása megjegyzésbe!</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-Lwg9TZe-xRKLpJLaTDO
+https://zsebtanar.hu/exercise/-LwgAUShD2-2_tkfF1yW
+https://zsebtanar.hu/exercise/-LwgC7_YHbgpmJxv8iEV
+https://zsebtanar.hu/exercise/-LwgHWcRkAeXibtBhf38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/34IpBCV
+http://bit.ly/2EKxQ6R
+http://bit.ly/34KtOGf
+http://bit.ly/2Q8gbvb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/ESEA0eTmH6g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kettes számrendszer 5. osztály,kettes számrendszer átváltás,kettes számrendszerből tizesbe,kettes számrendszer matematika,kettes számrendszer tizesbe,kettes számrendszer 10 átváltás,bináris számrendszer átváltás,bináris számrendszer,decimális bináris átváltás,bináris rendszer,tízes számrendszerből kettes számrendszerbe,tizes számrendszerből kettesbe,hexadecimális számrendszer,hexadecimális átváltás,hexadecimális decimális átváltás,kettes számrendszer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:16 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abszolút érték, ellentett</t>
   </si>
   <si>
@@ -260,6 +484,25 @@
 05:14:14</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LwvH4uibwqMSs4aMJl9
+https://zsebtanar.hu/exercise/-LwvHn8ov_V2UR_ascLO
+https://zsebtanar.hu/exercise/-LwvJ05qn5m1i0ov0eoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2EWCLBH
+http://bit.ly/2PTsPPI
+http://bit.ly/34R9NOb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/CYtEgw0B61s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abszolút érték kiszámítása,abszolút érték ábrázolása számegyenesen,abszolút érték ellentettje,ellentett abszolút érték,abszolút érték szabálya,abszolút értékű egész számok,0 abszolút értéke,abszolút érték,abszolút érték 5.osztály feladatok,ellentett érték,számok ellentettje abszolút értéke,számok ellentettje feladatok,a számok ellentettje abszolút értéke,számok abszolút értéke,számok abszolút értéke feladatok,a számok abszolút értéke,ellentett,számok ellentettje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:29 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Műveletek negatív számokkal</t>
   </si>
   <si>
@@ -278,6 +521,25 @@
 14:51:08</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LwvbKUzXtAME9_FRHEb
+https://zsebtanar.hu/exercise/-LwvhBbcKNE7mRgefOYl
+https://zsebtanar.hu/exercise/-LwvldPvAtS0ZTpGfY8v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/37djEjf
+http://bit.ly/378yYO4
+http://bit.ly/2Qe3VJI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/V2SYKnxrN3g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negatív számok osztása,negatív számok összeadása,negatív számok kivonása,negatív számok szorzása,negatív számok összeadása kivonása feladatok,negatív számokkal való műveletek,negatív számok kivonása és összeadása,negatív számok értelmezése,negatív számok feladatok 5. osztály,negatív számok gyakorlása,negatív számok összeadása kivonása,negatív számok 6 osztály,negatív számok 5 osztály,mínusz számok összeadása,minusz számok kivonása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:54 - 000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Műveleti sorrend</t>
   </si>
   <si>
@@ -294,6 +556,25 @@
     <t xml:space="preserve">05:14:25
 07:15:06
 09:09:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-Lx9_ippYFGx7Ki6Jjcw
+https://zsebtanar.hu/exercise/-Lx9abEBXKR47WQM9pHB
+https://zsebtanar.hu/exercise/-Lx9bPtCBD_NncIEzfWd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2SyEYeW
+http://bit.ly/2stCCDf
+http://bit.ly/2SwM1EM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/BOAQLO_-d5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">műveleti sorrend feladatok,műveleti sorrend 5. osztály,műveleti sorrend feladat,műveleti sorrend zárójel,műveleti sorrend feladatok 5. osztály,műveleti sorrend gyakorlása,műveletek sorrendje,műveletek sorrendje 5. osztály,műveletek sorrendje 6. osztály,műveletek sorrendje 4. osztály,műveletek sorrendje 5. osztály feladatok,műveletek sorrendje 6. osztály feladatok,műveletek sorrendje matematika,a műveletek sorrendje,műveleti sorrend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:15 - 000</t>
   </si>
   <si>
     <t xml:space="preserve">Közönséges törtek bevezetése. Racionális számok</t>
@@ -315,6 +596,31 @@
 07:53:06
 10:26:23
 14:13:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-Lxn3_9Ljb7_WLVObPMB
+https://zsebtanar.hu/exercise/-Lxn6_i7ZwLzJm4Dcndg
+https://zsebtanar.hu/exercise/-Lxn7UNeVNh-d9ZTVXst
+https://zsebtanar.hu/exercise/-LxnDSg60ilo-3B1rmcr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2QQF7aS
+http://bit.ly/39BHFSW
+http://bit.ly/2sBsb0J
+http://bit.ly/2Qq7ga3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/7ATwDj0EX4Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">közönséges törtek,matek törtek,racionális számok,racionális törtek,számláló és nevező fogalma,tört ábrázolása számegyenesen,tört alak,tört alakba váltás,tört alakban írt egész szám,törtek 5. osztály gyakorlás,törtek 5. osztály,törtek ábrázolása számegyenesen 5. osztály,törtek abszolút értéke,törtek egyszerűen,törtek fogalma,törtek részei,törtek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:01 - 008
+3:45 - 016
+9:04 - 013
+10:38 - 004
+13:45 - 012</t>
   </si>
   <si>
     <t xml:space="preserve">Közönséges törtek bővítése, egyszerűsítése, összehasonlítása</t>
@@ -339,6 +645,32 @@
 14:50:17
 17:06:02
 21:40:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LyHvwBEybV-rjIknaw6
+https://zsebtanar.hu/exercise/-LyHxM0D-XO9ZFNMOval
+https://zsebtanar.hu/exercise/-LyI8d5oZXHBQg1KtSAq
+https://zsebtanar.hu/exercise/-LyIA-HGfkk2codVLq50
+https://zsebtanar.hu/exercise/-LyIBxokSlD6qHTSXMvR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2FCW03A
+http://bit.ly/2TcaOhR
+http://bit.ly/2R9ao94
+http://bit.ly/37ZjUCS
+http://bit.ly/2TdsoBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/ddPaUJu9J6I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a törtek bővítése,a törtek egyszerűsítése,a törtek közös nevezőre hozása,a törtek összehasonlítása,közönséges törtek bővítése,tört bővítése szabály,tört egyszerűsítése,törtek bővítése 5 osztály,törtek bővítése és egyszerűsítése,törtek bővítése,törtek csökkenő sorrend,törtek egyszerűsítése és bővítése,törtek egyszerűsítése szabály,törtek közös nevezőre hozása feladatok,törtek közös nevezőre hozása,törtek melyik a nagyobb,törtek növekvő sorrendben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:44 - 015
+3:51 - 007
+4:56 - 010
+12:30 LKKT</t>
   </si>
   <si>
     <t xml:space="preserve">Közönséges törtek összeadása, kivonása, közös nevező</t>
@@ -366,6 +698,35 @@
 29:08:08
 40:16:08
 42:36:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LytJtGCiaget2e7MQB_
+https://zsebtanar.hu/exercise/-LytL9eWoR6dYm4pl0P3
+https://zsebtanar.hu/exercise/-LytMIMW3u2-ylefPsEf
+https://zsebtanar.hu/exercise/-LytTEk8uhv1f0yD-jIF
+https://zsebtanar.hu/exercise/-LytVbhE4dVaHhW0RZN6
+https://zsebtanar.hu/exercise/-LytWV7EyVib07TbN6Fp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2tuDk3K
+http://bit.ly/2NAfqdW
+http://bit.ly/2v3xiYn
+http://bit.ly/37d5r6k
+http://bit.ly/2G34eT0
+http://bit.ly/38dwsq6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/iPSiKpT8s-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 tört összeadása,közönséges törtek összeadása,különböző nevezőjű törtek összeadása,több tört összeadása,tört és egész szám összeadása,tört összeadása,törtek és egész számok összeadása,törtek kivonása és összeadása,törtek összeadása és kivonása,törtek összeadása,zárójeles törtek összeadása,különböző nevezőjű törtek kivonása,törtek kivonása egész számból,törtek kivonása,törtek alapműveletek,törtek műveleti sorrend,törtek pillangós módszer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:26 - 016
+7:46 - 013
+13:02 - 010
+18:09 - 014
+22:50 - 012</t>
   </si>
   <si>
     <t xml:space="preserve">Közönséges törtek szorzása, osztása, reciproka</t>
@@ -398,6 +759,36 @@
 28:19:01</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-LzKqFx_N5a708cCoBni
+https://zsebtanar.hu/exercise/-LzKrqYx-HYB7HtSxWhf
+https://zsebtanar.hu/exercise/-LzPpy6ZMc39hZTkgnAS
+https://zsebtanar.hu/exercise/-LzProqmBdeTr1NK2ydm
+https://zsebtanar.hu/exercise/-LzPu00ZThkEwrcU36N3
+https://zsebtanar.hu/exercise/-LzPz86iGlwPWTVAaq0r
+https://zsebtanar.hu/exercise/-LzQ-iSNKgFLXY9j00oC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2RNQFfs
+http://bit.ly/2ROdKPp
+http://bit.ly/30QEIKl
+http://bit.ly/2GkHoXh
+http://bit.ly/2RptUj9
+http://bit.ly/38vb3sK
+http://bit.ly/2Rpw6XV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/YugzJW0S58Q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reciprok osztás törttel,reciprok fogalma,reciprok számítás,reciproka fogalma,törtek reciproka,3 tört osztása,3 tört szorzása,tört és egész szám szorzása,tört osztása egész számmal,tört osztása törttel,tört reciproka,tört számok osztása,tört törttel való szorzása,törtek hányadosa,törtek osztása egész számmal,törtek osztása szorzása,törtek osztása tört számmal,törtek osztása,törtek szorzása osztása,törtek szorzása,törtek törttel való szorzása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:56 - 012
+12:21 - 013
+18:03 - 014
+18:17 - 017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vegyes számok</t>
   </si>
   <si>
@@ -420,6 +811,32 @@
 22:29:01
 29:55:20
 34:02:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M-0QPakJ9n_SbzN_qsC
+https://zsebtanar.hu/exercise/-M-0S4nppzVjzYLXf6NT
+https://zsebtanar.hu/exercise/-M-0XYMeeYlLE5iouwQD
+https://zsebtanar.hu/exercise/-M-0_24cLWC_kccHazj4
+https://zsebtanar.hu/exercise/-M-0eHnxvzX6kjbfU6qN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2Og6cUn
+http://bit.ly/36PDctf
+http://bit.ly/2OkPTG9
+http://bit.ly/2Oi9CpW
+http://bit.ly/37PoDaq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/kxPyS_uU6Rk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegyes törtek kivonása,vegyes számok törté alakítása,vegyes számok összeadása,vegyes számok kivonása,vegyes számok tört alakban,vegyes törtek,vegyes törtek szorzása,vegyes törtek osztása,vegyes tört átalakítása törtté,vegyes tört szorzása egész számmal,vegyes tört átalakítása,vegyes törtből tört,vegyes tört szorzása vegyes törttel,vegyes tört egyszerűsítése,tört átalakítása vegyes törtté,törtek vegyes szám alakja,törtek vegyes számmá alakítása,vegyes számok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:09 - 017
+4:12 - 014
+24:22 - 018
+27:59 - 013</t>
   </si>
   <si>
     <t xml:space="preserve">Tizedes törtek</t>
@@ -456,6 +873,41 @@
 48:47:08
 52:40:10
 1:03:25:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M-cGQNt4q-WkFpDGUel
+https://zsebtanar.hu/exercise/-M-cIiVOHGvXgfAkwUyL
+https://zsebtanar.hu/exercise/-M-cYmR6NdSg-lsexm_M
+https://zsebtanar.hu/exercise/-M-c_LMJyuiMffYhvWrO
+https://zsebtanar.hu/exercise/-M-cbz4jGwj1RikpYvIl
+https://zsebtanar.hu/exercise/-M-ceZ2bTom_I4rO7L4t
+https://zsebtanar.hu/exercise/-M-cgq0h96ivJ_EM-4m6
+https://zsebtanar.hu/exercise/-M-cjquybiVXDVy90ITs
+https://zsebtanar.hu/exercise/-M-cmnjLlUvc_KDWIlJa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2OAOmf6
+http://bit.ly/2w2kWAd
+http://bit.ly/38dsq1k
+http://bit.ly/2SykyB5
+http://bit.ly/2OEI3r8
+http://bit.ly/3brPfka
+http://bit.ly/2vewlMS
+http://bit.ly/39kWqsg
+http://bit.ly/2OFAArx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/PFSDHTMf0wQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">közönséges tört átalakítása tizedes törtté,tizedes tört szorzása törttel,tört átalakítása,tört átváltása tizedes törtté,tört átváltása,tört egész számmá alakítása,tört és tizedes tört összeadása,tört szorzása tizedes törttel,tizedes törtek a számegyenesen,tört szám átváltása tizedes törtté,tört tizedes törtté alakítása,tizedes tört szorzása tizedes törttel,törtek felírása tizedes tört alakban,végtelen tizedes tört törtté alakítása,tizedes tört,tizedes törtek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:17 - 001
+7:17 - 016
+14:19 - 009
+24:14 - 005
+35:39 - 007</t>
   </si>
   <si>
     <t xml:space="preserve">Szöveges feladatok törtekkel</t>
@@ -509,6 +961,51 @@
 48:27:03</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M0BBEAEnyC0efRGhw-V
+https://zsebtanar.hu/exercise/-M0BCf2hEsuvGKmj3J2G
+https://zsebtanar.hu/exercise/-M0BDs-kyNPBGEb6QFpW
+https://zsebtanar.hu/exercise/-M0BE_4lyj2EWtBMzORx
+https://zsebtanar.hu/exercise/-M0BFbUJ1s7BSnaS8bmb
+https://zsebtanar.hu/exercise/-M0BHT06Lo7ishLEBZzj
+https://zsebtanar.hu/exercise/-M0BI1edVXLmba4JWJ3g
+https://zsebtanar.hu/exercise/-M0BIfawEX6BUx8dWFpd
+https://zsebtanar.hu/exercise/-M0BJooaAUeQWANPzkxo
+https://zsebtanar.hu/exercise/-M0BKf5SLYyMy934qrnF
+https://zsebtanar.hu/exercise/-M0BLOVLYo_3dJqQnJvG
+https://zsebtanar.hu/exercise/-M0BM8VCHR3cRk5XC3bN
+https://zsebtanar.hu/exercise/-M0BOV9hU3OITssNLpN3
+https://zsebtanar.hu/exercise/-M0BOxu2lxjosOfQoQP6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/2SRxAdb
+http://bit.ly/2SvBtFx
+http://bit.ly/39Ehieq
+http://bit.ly/2OX88S2
+http://bit.ly/2UWSPgm
+http://bit.ly/2u5NPuK
+http://bit.ly/39Cfd2p
+http://bit.ly/2UYLpJh
+http://bit.ly/38zadLV
+http://bit.ly/3bGK3sM
+http://bit.ly/2OYwo6n
+http://bit.ly/2u5Ey5S
+http://bit.ly/2uFbP8o
+http://bit.ly/2HqMHEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/QAowehB_-y8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">szöveges feladatok,szöveges feladatok 5. osztály,szöveges feladatok megoldása,szöveges feladatok megoldása törtekkel,szöveges feladatok megoldása törtekkel 5. osztály,szöveges feladat törtekkel,szöveges feladat lépései,szöveges feladat megoldása,törtek szöveges feladatok 5. osztály,törtek feladatok 5. osztály,törtek gyakorló feladatok 5.osztály,szöveges feladatok megoldása törtekkel 5.osztály,matek szöveges feladatok 5.osztály,keveréses szöveges feladatok 5. osztály</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:17 - 015
+11:44 - 019
+16:16 - 018
+19:45 - 020
+26:01 - 017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mértékegységek átváltása</t>
   </si>
   <si>
@@ -545,10 +1042,59 @@
 39:32:10</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M193lWr-cTdaF_ra5lW
+https://zsebtanar.hu/exercise/-M198ZG1SAfOZxvf1zXI
+https://zsebtanar.hu/exercise/-M19AtZOq2pPHdcH3lSZ
+https://zsebtanar.hu/exercise/-M19ClnxyD0BEU_2-CPi
+https://zsebtanar.hu/exercise/-M19DzVkzePgD4oONXcE
+https://zsebtanar.hu/exercise/-M19F2ddf84lmpJEtZ8v
+https://zsebtanar.hu/exercise/-M19HYpasteU6mHtLq40
+https://zsebtanar.hu/exercise/-M19KNFHHD4UJcZfanD-
+https://zsebtanar.hu/exercise/-M19NG4typjQmqFnD6g1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/3981JvA
+http://bit.ly/2TsZA7g
+http://bit.ly/2wfRre5
+http://bit.ly/3abivKh
+http://bit.ly/2Pw3gUq
+http://bit.ly/2wUIU0K
+http://bit.ly/399JtSv
+http://bit.ly/3adCIPO
+http://bit.ly/3admAOd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/f4fEpztGDH0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mértékegységek,mértékegységek tanítása,mértékegységek átváltása,mértékegységek története,mértékegység váltás,mértékegység átváltás tanítása,mértékegység átváltás 5. osztály,mértékegység átváltások,mértékegység feladatok 5.osztályosoknak,hosszúság mértékegység átváltás,hosszúság mértékegység,mértékegység tanítása,tömeg mértékegység átváltás,idő átváltása,hosszúság átváltása,tömeg átváltása,az si mértékegységek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:25 - 020
+20:15 - 021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hiányzó számláló, nevező pótlása</t>
   </si>
   <si>
     <t xml:space="preserve">1. Hiányzó számláló, nevező pótlása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M1iDuIaqCf62aSO2Kv-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/38qTiKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/D12igcEzJh8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pótold a nevezőt,hiányzó nevező,nevező pótlása,pótold a számlálót,számláló pótlása,hiányzó számláló,közönséges törtek bővítése,törtek egyszerűsítése bővítése,közönséges törtek egyszerűsítése,bővítés,egyszerűsítés,tört bővítése,tört egyszerűsítése,tört egyszerűsítés,törtek bővítése,törtek egyszerűsítése,egyszerűsítés matek,egyszerűsítés törtekkel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:19 - 016
+3:49 - 019
+5:07 - 010</t>
   </si>
   <si>
     <t xml:space="preserve">Geometria bevezetés</t>
@@ -584,6 +1130,32 @@
 23:29:14</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M2_TAUQ5g6sdUhDpeYt
+https://zsebtanar.hu/exercise/-M2_UNL0rgptR_DrjbDF
+https://zsebtanar.hu/exercise/-M2aW6a6pidF7Q83Sg6G
+https://zsebtanar.hu/exercise/-M2aZ3BO6-eTk5O0cfOL
+https://zsebtanar.hu/exercise/-M2aZaZKaPSZRNDCrF3Q
+https://zsebtanar.hu/exercise/-M2aaLjyEaMf9xGlQeBT
+https://zsebtanar.hu/exercise/-M2abXY_VnQM19wFxm0P
+https://zsebtanar.hu/exercise/-M2acKCi72bgM1j6jgMw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://bit.ly/3deJU0q
+http://bit.ly/2xBUKgq
+http://bit.ly/3b3OPz4
+http://bit.ly/3d80leH
+http://bit.ly/39SfcIe
+http://bit.ly/2ISvuFc
+http://bit.ly/2IT9j1y
+http://bit.ly/33pw4Ut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/2JabIVJKbNY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geometriai alapfogalmak,geometria 5. osztály,geometria alapfogalmak,geometria 5. osztály feladatok,pont fogalma,egyenes fogalma,sík fogalma,félsík fogalma,tér fogalma,kitérő egyenes,egyenes és részei,egyenes félegyenes szakasz,egyenes kölcsönös helyzete,egyenes metszéspontja,az egyenes fogalma,2 egyenes távolsága,egyenesek kölcsönös helyzete,kitérő egyenesek,metsző egyenesek,párhuzamos egyenesek,geometria 5. osztály bevezetés</t>
+  </si>
+  <si>
     <t xml:space="preserve">Síkidomok, sokszögek, testek</t>
   </si>
   <si>
@@ -617,6 +1189,36 @@
 28:19:08</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M3K1GQ4vkp-jGBrhd95
+https://zsebtanar.hu/exercise/-M3K2x-65MEWTuZbxs4t
+https://zsebtanar.hu/exercise/-M3K3jW20wIQTZBYOaHO
+https://zsebtanar.hu/exercise/-M3KDyxe3gkKPnGraljr
+https://zsebtanar.hu/exercise/-M3KGZBIu3IYPRceXEw0
+https://zsebtanar.hu/exercise/-M3KJASB3L6JEa9Kwf7K
+https://zsebtanar.hu/exercise/-M3LydXgMnpdmVvI0CNS
+https://zsebtanar.hu/exercise/-M3M24NKBDVqA9Vt0lwp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2QLz9sM
+https://bit.ly/2JhMuFa
+https://bit.ly/3bpKW7P
+https://bit.ly/3dxR7Zk
+https://bit.ly/39nBIaS
+https://bit.ly/2UkUmfi
+https://bit.ly/3apMRt6
+https://bit.ly/2UjBNIf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/vvMsVp0bNdw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">konkáv jelentése,konkáv négyszög,konkáv síkidom,konvex definíció,konvex konkáv 5. osztály,konvex konkáv jelentése,konvex konkáv,konvex síkidom,konvex síkidomok,konvex sokszög,lapátló jelentése,síkidom jelentése,síkidomok 5 osztály,síkidomok átlóinak száma,síkidomok sokszögek 5. osztály,sokszög átló számítás,sokszög átlóinak száma,sokszög fogalma,sokszög összes átlója,sokszögek fajtái,sokszögek tulajdonságai,testátló fogalma,testátló jelentése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:36 - 026
+24:10 - 024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Szögfajták, nevezetes szögpárok</t>
   </si>
   <si>
@@ -650,7 +1252,52 @@
 29:58:25</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M3ifcb2tggBdyv3qh4H
+https://zsebtanar.hu/exercise/-M3ihDJOgQ06jkNKxoaN
+https://zsebtanar.hu/exercise/-M3ilWghjke9wE-bD4oT
+https://zsebtanar.hu/exercise/-M3imvoddUr9XzbXf-H8
+https://zsebtanar.hu/exercise/-M3intdKVCz_be3KTWre
+https://zsebtanar.hu/exercise/-M3ipPODyNpOm1EizBzS
+https://zsebtanar.hu/exercise/-M3nbFzPnGQ2sjbXwxe5
+https://zsebtanar.hu/exercise/-M3nd6jjNcR6lj-xFiSs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/3bHJPjZ
+https://bit.ly/2Ut0xOw
+https://bit.ly/2UtNUCD
+https://bit.ly/2xCR7H0
+https://bit.ly/2Uy2Foh
+https://bit.ly/33VRFUw
+https://bit.ly/3bAuLVo
+https://bit.ly/3aAh5JU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/EPgx_HgWDhA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">szögfajták,nevezetes szögpárok 5 osztály,szögtípusok,nullszög,hegyesszög,derékszög jelentése,tompaszög,egyenesszög,homorúszög,teljesszög,konkáv szög jelentése,konvex szög fogalma,mellékszög,társszög,egyállású szögek,fordított állású szögek,váltószögek,csúcsszögek,nevezetes szögpárok gyakorló feladat,pótszögek,szögperc,szögmásodperc,szögek átváltása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:31 - 025
+15:13 - 022
+18:55 - 006
+23:10 - 020
+24:57 - 009</t>
+  </si>
+  <si>
     <t xml:space="preserve">Négyzetek, téglalapok - igaz-hamis állítások</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M4S3kEI-UeWArq9WLm-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2XlsSYJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/J_7HJoq4lg0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">négyzet,téglalap,a négyzet is téglalap,a négyzet tulajdonságai,négyzet definíciója,négyzet és téglalap tulajdonságai,négyzet és téglalap,négyzet is téglalap,négyzet jellemzői,négyzet oldalai,a négyzet,négyzet tulajdonságai,a téglalap tulajdonságai,a téglalap négyzet,téglalap átlója,téglalap átló,téglalap definíciója,téglalap és négyzet,téglalap fogalma,téglalap feladatok,téglalap jellemzői,téglalap négyzet,téglalap oldalai</t>
   </si>
   <si>
     <t xml:space="preserve">Hány darab négyzet és téglalap látható a képen?</t>
@@ -668,10 +1315,60 @@
 07:14:07</t>
   </si>
   <si>
+    <t xml:space="preserve">feladat szétszed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M4X4MBNd366MUr4RpKk
+https://zsebtanar.hu/exercise/-M4X4MBNd366MUr4RpKk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/34qsRnQ
+https://bit.ly/34qsRnQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/_waVY1XwekM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">négyzet,téglalap,négyzet és téglalap,négyzet oldalai,a négyzet,téglalap és négyzet,téglalap feladatok,téglalap négyzet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Négyzet területe, kerülete</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M4gYxTnO82bf6CscfvB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2JXniE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Vf70TPSP8L8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">négyzet területe,a négyzet kerülete,a négyzet területe,a négyzet tulajdonságai,négyzet definíciója,négyzet és téglalap területe,négyzet jellemzői,négyzet kerülete,négyzet kerület terület,négyzet kerület,négyzet téglalap területe,négyzet téglalap,négyzet m átváltás,négyzet oldalainak kiszámítása területből,négyzet oldalai,a négyzet,négyzet tulajdonságai,négyzet téglalap kerülete területe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:35 - 022
+4:16 - 020</t>
+  </si>
+  <si>
     <t xml:space="preserve">Téglalap területe, kerülete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M4ggiwxZcEXa5pbP-lO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2xo1FKn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Nt9vhZFFiLs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">téglalap területe,téglalap négyzet kerülete,a téglalap kerülete,a téglalap területe,téglalap b oldalának kiszámítása,téglalap és négyzet területe,téglalap és négyzet kerülete,téglalap hiányzó oldalának kiszámítása,téglalap ismeretlen oldalának kiszámítása,téglalap kerülete,téglalap területszámítás,téglalap kerület számítás,téglalap négyzet kerülete területe,téglalap oldalainak kiszámítása,téglalap területe 5. osztály,téglalap terület,téglalap területe kerülete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:11 - 029
+3:07 - 022
+6:26 - 007</t>
   </si>
   <si>
     <t xml:space="preserve">Téglalap területe, kerülete - szöveges feladatok</t>
@@ -695,13 +1392,86 @@
 09:32:29</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M505NQwWIpTe-LdJ1a3
+https://zsebtanar.hu/exercise/-M506e1fJleJrt7SQqjj
+https://zsebtanar.hu/exercise/-M507kaEjEDcHZZDuKZj
+https://zsebtanar.hu/exercise/-M508qoPPOQGWvPhIAzy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2xpgUDb
+https://bit.ly/2RIOuuz
+https://bit.ly/34CEyYW
+https://bit.ly/2VdjpRU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Ihc8eSQu6Aw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">téglalap területe,a téglalap kerülete,téglalap b oldalának kiszámítása,téglalap és négyzet területe,téglalap és négyzet kerülete,téglalap hiányzó oldalának kiszámítása,téglalap ismeretlen oldalának kiszámítása,téglalap kerülete,téglalap oldalainak kiszámítása,téglalap területe 5. osztály,téglalap terület,téglalap területe kerülete,téglalap területe szöveges feladat,téglalap kerülete szöveges feladat,téglalap szöveges feladat,téglalap szöveges feladat 5. osztály</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:18 - 030
+3:41 - 014
+3:53 - 020
+6:50 - 022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Téglatest, kocka - igaz-hamis állítások</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M5ECo8VimuWop7B5oYs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2XK95CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/eZE5CVbTKaY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kocka és téglatest,kocka éle,kocka éleinek kiszámítása,kocka jellemzői,kocka jellemzése,kocka kocka,kocka matematika,kocka matek,kocka téglatest,kocka 5. osztály,téglatest kocka 4. osztály,téglatest definíciója,téglatest és kocka,téglatest jellemzői,téglatest kocka,téglatest kocka fogalma,téglatest szabályok,téglatest tulajdonságai,téglatest 5. osztály,téglatest kocka 5. osztály</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:33 - 027</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kocka felszíne, térfogata</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M5V1IxGGsrFLiRmzA7C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2KpBsyg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/qLukwH_rE-U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kocka felszíne,kocka alapterülete,a kocka felszíne,a kocka felszíne és térfogata,a kocka térfogata,kocka éleinek kiszámítása,kocka és téglatest térfogata,kocka felszíne térfogata,kocka felszíne kiszámítása,kocka felszíne és térfogata,kocka jellemzői,kocka jellemzése,kocka kerülete,kocka matematika,kocka matek,kocka oldalainak kiszámítása,kocka oldal felszine,kocka térfogata,kocka téglatest,kocka területe,kocka téglatest felszíne térfogata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:19 - 032
+0:54 - 029
+4:43 - 022</t>
+  </si>
+  <si>
     <t xml:space="preserve">Téglatest felszíne, térfogata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M5_EOFds243ckYmaWq-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2yCZfb0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/tAR5uLJBRiw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">téglatest felszíne,téglatest alapterülete,a téglatest felszíne,a téglatest felszíne és térfogata,a téglatest térfogata,téglatest éleinek kiszámítása,téglatest felszíne térfogata,téglatest felszíne kiszámítása,téglatest felszíne és térfogata,téglatest jellemzői,téglatest jellemzése,téglatest kerülete,téglatest matematika,téglatest matek,téglatest oldalainak kiszámítása,téglatest oldal felszine,téglatest térfogata,kocka téglatest,téglatest területe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:13 - 032
+0:48 - 030
+4:19 - 022</t>
   </si>
   <si>
     <t xml:space="preserve">Kocka, téglatest - szöveges feladatok</t>
@@ -725,7 +1495,46 @@
 13:17:16</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M5eP6RSj5cNGER4K5IH
+https://zsebtanar.hu/exercise/-M5eQ2FM-FBNrYkXUzUb
+https://zsebtanar.hu/exercise/-M5eT6CQcLxUYSBlJGS8
+https://zsebtanar.hu/exercise/-M5eU93TGrTxVxGKt2HX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/3cGFe2a
+https://bit.ly/3cFEUkj
+https://bit.ly/3cHc1UF
+https://bit.ly/2Y2m178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/RzYgrga1kWk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kocka és téglatest szöveges feladatok,kocka testhálózata,téglatest hálózata,kocka szöveges feladat,téglatest szöveges feladat,kocka matematika,kocka matek,kocka téglatest,kocka 5. osztály,téglatest kocka 5. osztály,téglatest térfogata,téglatest felszíne,téglatest és kocka,téglatest kocka,téglatest 5. osztály</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:00 - 039
+1:47 - 034
+2:08 - 007</t>
+  </si>
+  <si>
     <t xml:space="preserve">Négyzetszámok, köbszámok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M5jWcVNvAcqbeW1oZGy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2S3U76K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/de8QpgBsre8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">négyzetszámok,köbszámok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:18 - 029
+0:45 - 033</t>
   </si>
   <si>
     <t xml:space="preserve">Kör és gömb részei - szöveges feladatok</t>
@@ -752,10 +1561,69 @@
 10:21:13</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M689vIlyDGwKa6DGfuT
+https://zsebtanar.hu/exercise/-M68AvQX4v1_iilOHbis
+https://zsebtanar.hu/exercise/-M68CANY7YuBG3LD2X2V
+https://zsebtanar.hu/exercise/-M68CsjOWeczr4sTJT46
+https://zsebtanar.hu/exercise/-M68FRLlGjXcKMgXGZj3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/35p0qra
+https://bit.ly/2yWQDw2
+https://bit.ly/35gIoqU
+https://bit.ly/2VQAVf7
+https://bit.ly/2SkTfLe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/F86_RQ69JXs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gömb sugara,kör részei,gömb átmérője,kör matematika 5. osztály,gömb részei 5. osztály,húr jelentése,szelő jelentése,körszelet jelentése,körcikk jelentése,kör középpontja,kör sugara,kör átmérője,kör érintője,kör szelője,körlap,körgyűrű jelentése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:02 - 024</t>
+  </si>
+  <si>
     <t xml:space="preserve">Terület átváltása</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M6NpqzOBmIkMLREGP3H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2yn97WD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/zSeE9Nv1fYo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">területszámítás,terület mérése,terület fogalma 4. osztály,területszámítás 3. osztály,terület mértékegységei,terület mértékváltás,a terület mérése,a terület mértékegységei,a területmérés mértékegységei,terület átváltás feladatok,terület mértékegység átváltás,mértékegység átváltás 5. osztály,négyzetméter átváltás,mértékegység átváltás terület</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:24 - 022
+1:37 - 029
+4:11 - 020
+4:25 - 031</t>
+  </si>
+  <si>
     <t xml:space="preserve">Térfogat átváltása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M6wyk_aYbJn4Xtd1G-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/2SSLGvv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/UlwJ5pKYVXU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">térfogat mértékegysége,térfogatszámítás,térfogat átváltás,térfogat és űrtartalom,térfogat mértékváltás,a térfogat mértékegysége,térfogat átváltás literre,térfogat és űrmérték átváltás,térfogat és űrtartalom átváltás,térfogat mértékegység átváltás,térfogat 5. osztály,térfogat űrtartalom átváltás,térfogat váltószámok,ürtartalom átváltás,űrtartalom átváltása térfogatra,űrtartalom térfogat,űrtartalom térfogat átváltás,űrtartalom táblázat,űrtartalom váltószámok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:32 - 038
+1:37 - 033
+1:55 - 022
+10:40 - 020</t>
   </si>
   <si>
     <t xml:space="preserve">Koordináta-rendszer</t>
@@ -785,10 +1653,52 @@
 16:14:23</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M82QCekq_fhPOZ2x_Nm
+https://zsebtanar.hu/exercise/-M82TShisQC9ANUpu6j9
+https://zsebtanar.hu/exercise/-M82bHpkVgVZmQvB3oFa
+https://zsebtanar.hu/exercise/-M83WhxnCb4wO5-3Z39Y
+https://zsebtanar.hu/exercise/-M84Gn7ofDjlQSC2WOim
+https://zsebtanar.hu/exercise/-M84I7NvmrwGd2OBlwxS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/3cYEOEZ
+https://bit.ly/2XsXvKe
+https://bit.ly/2WZEBMi
+https://bit.ly/2yqw9vQ
+https://bit.ly/3e99HGI
+https://bit.ly/2WXsRtx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/Qr6r5MCnr8Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koordináta rendszer,koordináta rendszer 5. osztály,a koordináta rendszer,a derékszögű koordináta rendszer,koordináta ábrázolás,pontok ábrázolása koordináta rendszerben,derékszögű koordináta rendszer,descartes féle koordináta rendszer,koordináta rendszer feladatok,koordinátasík,síknegyed,René Descartes,polárkoordináta rendszer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:24 - 004
+6:58 - 012
+10:45 - 026</t>
+  </si>
+  <si>
     <t xml:space="preserve">A koronavírus matematikája</t>
   </si>
   <si>
     <t xml:space="preserve">Járványmodellek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://zsebtanar.hu/exercise/-M9Ma7lItlNZchewRohy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bit.ly/3hbGcGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/GmXWs6dHS3c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">koronavírus,matematika,covid 19 világjárvány,koronavírus-járvány,vírus,járvány,járványmodellek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:08 - 040</t>
   </si>
   <si>
     <t xml:space="preserve">1. Szám meghatározása szöveg alapján </t>
@@ -1235,7 +2145,7 @@
     <numFmt numFmtId="165" formatCode="HH:MM:SS"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1260,6 +2170,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1307,13 +2224,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1324,12 +2245,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1353,337 +2282,609 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="48.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="53.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="48.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="56.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="48.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="79.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>49</v>
+        <v>101</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>147</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>74</v>
+        <v>156</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="79.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,33 +2892,63 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>82</v>
+        <v>174</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="102.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,16 +2956,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>86</v>
+        <v>183</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="158.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,16 +2988,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>90</v>
+        <v>192</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="102.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,33 +3020,63 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>95</v>
+        <v>210</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="5" t="n">
+        <v>211</v>
+      </c>
+      <c r="D24" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="7" t="n">
         <v>0.316111111111111</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,16 +3084,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>100</v>
+        <v>217</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,16 +3113,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>104</v>
+        <v>225</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,33 +3145,60 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="79.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>109</v>
+        <v>243</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="5" t="n">
+        <v>243</v>
+      </c>
+      <c r="D28" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" s="7" t="n">
         <v>0.118946759259259</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,135 +3206,255 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>248</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="79.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>114</v>
+        <v>257</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="5" t="n">
+        <v>257</v>
+      </c>
+      <c r="D30" s="7" t="n">
         <v>0.00295138888888889</v>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" s="7" t="n">
         <v>0.33125</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>115</v>
+        <v>263</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="5" t="n">
+        <v>263</v>
+      </c>
+      <c r="D31" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E31" s="5" t="n">
+      <c r="E31" s="7" t="n">
         <v>0.297291666666667</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>269</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="79.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>120</v>
+        <v>278</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D33" s="5" t="n">
+        <v>278</v>
+      </c>
+      <c r="D33" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E33" s="5" t="n">
+      <c r="E33" s="7" t="n">
         <v>0.137534722222222</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="79.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>121</v>
+        <v>284</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="5" t="n">
+        <v>284</v>
+      </c>
+      <c r="D34" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E34" s="5" t="n">
+      <c r="E34" s="7" t="n">
         <v>0.377407407407407</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>122</v>
+        <v>290</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="5" t="n">
+        <v>290</v>
+      </c>
+      <c r="D35" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E35" s="5" t="n">
+      <c r="E35" s="7" t="n">
         <v>0.43912037037037</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>126</v>
+        <v>296</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,16 +3462,31 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>127</v>
+        <v>305</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" s="5" t="n">
+        <v>305</v>
+      </c>
+      <c r="D37" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E37" s="5" t="n">
+      <c r="E37" s="7" t="n">
         <v>0.096724537037037</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,50 +3494,95 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>311</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>132</v>
+        <v>320</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" s="5" t="n">
+        <v>320</v>
+      </c>
+      <c r="D39" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E39" s="5" t="n">
+      <c r="E39" s="7" t="n">
         <v>0.404444444444444</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>133</v>
+        <v>326</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="5" t="n">
+        <v>326</v>
+      </c>
+      <c r="D40" s="7" t="n">
         <v>0.0175462962962963</v>
       </c>
-      <c r="E40" s="5" t="n">
+      <c r="E40" s="7" t="n">
         <v>0.64931712962963</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2065,33 +3590,63 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>332</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>138</v>
+        <v>341</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="D42" s="5" t="n">
+        <v>342</v>
+      </c>
+      <c r="D42" s="7" t="n">
         <v>0.00296296296296296</v>
       </c>
-      <c r="E42" s="5" t="n">
+      <c r="E42" s="7" t="n">
         <v>0.148819444444444</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2116,1411 +3671,1421 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="6" t="e">
+        <v>348</v>
+      </c>
+      <c r="B1" s="9" t="e">
         <f aca="false">HLOOKUP(A1,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="6" t="e">
+        <v>349</v>
+      </c>
+      <c r="B2" s="9" t="e">
         <f aca="false">HLOOKUP(A2,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="6" t="e">
+        <v>350</v>
+      </c>
+      <c r="B3" s="9" t="e">
         <f aca="false">HLOOKUP(A3,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="6" t="e">
+        <v>351</v>
+      </c>
+      <c r="B4" s="9" t="e">
         <f aca="false">HLOOKUP(A4,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="6" t="e">
+        <v>352</v>
+      </c>
+      <c r="B5" s="9" t="e">
         <f aca="false">HLOOKUP(A5,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="6" t="e">
+        <v>353</v>
+      </c>
+      <c r="B6" s="9" t="e">
         <f aca="false">HLOOKUP(A6,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="6" t="e">
+        <v>354</v>
+      </c>
+      <c r="B7" s="9" t="e">
         <f aca="false">HLOOKUP(A7,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="6" t="e">
+        <v>355</v>
+      </c>
+      <c r="B8" s="9" t="e">
         <f aca="false">HLOOKUP(A8,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B9" s="6" t="e">
+        <v>356</v>
+      </c>
+      <c r="B9" s="9" t="e">
         <f aca="false">HLOOKUP(A9,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="6" t="e">
+        <v>357</v>
+      </c>
+      <c r="B10" s="9" t="e">
         <f aca="false">HLOOKUP(A10,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="6" t="e">
+        <v>358</v>
+      </c>
+      <c r="B11" s="9" t="e">
         <f aca="false">HLOOKUP(A11,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="6" t="e">
+        <v>359</v>
+      </c>
+      <c r="B12" s="9" t="e">
         <f aca="false">HLOOKUP(A12,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B13" s="6" t="e">
+        <v>360</v>
+      </c>
+      <c r="B13" s="9" t="e">
         <f aca="false">HLOOKUP(A13,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="6" t="e">
+        <v>361</v>
+      </c>
+      <c r="B14" s="9" t="e">
         <f aca="false">HLOOKUP(A14,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" s="6" t="e">
+        <v>362</v>
+      </c>
+      <c r="B15" s="9" t="e">
         <f aca="false">HLOOKUP(A15,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="6" t="e">
+        <v>363</v>
+      </c>
+      <c r="B16" s="9" t="e">
         <f aca="false">HLOOKUP(A16,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="6" t="e">
+        <v>364</v>
+      </c>
+      <c r="B17" s="9" t="e">
         <f aca="false">HLOOKUP(A17,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B18" s="6" t="e">
+        <v>365</v>
+      </c>
+      <c r="B18" s="9" t="e">
         <f aca="false">HLOOKUP(A18,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B19" s="6" t="e">
+        <v>366</v>
+      </c>
+      <c r="B19" s="9" t="e">
         <f aca="false">HLOOKUP(A19,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B20" s="6" t="e">
+        <v>367</v>
+      </c>
+      <c r="B20" s="9" t="e">
         <f aca="false">HLOOKUP(A20,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B21" s="6" t="e">
+        <v>368</v>
+      </c>
+      <c r="B21" s="9" t="e">
         <f aca="false">HLOOKUP(A21,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B22" s="6" t="e">
+        <v>369</v>
+      </c>
+      <c r="B22" s="9" t="e">
         <f aca="false">HLOOKUP(A22,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B23" s="6" t="e">
+        <v>370</v>
+      </c>
+      <c r="B23" s="9" t="e">
         <f aca="false">HLOOKUP(A23,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B24" s="6" t="e">
+        <v>371</v>
+      </c>
+      <c r="B24" s="9" t="e">
         <f aca="false">HLOOKUP(A24,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B25" s="6" t="e">
+        <v>372</v>
+      </c>
+      <c r="B25" s="9" t="e">
         <f aca="false">HLOOKUP(A25,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B26" s="6" t="e">
+        <v>373</v>
+      </c>
+      <c r="B26" s="9" t="e">
         <f aca="false">HLOOKUP(A26,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B27" s="6" t="e">
+        <v>374</v>
+      </c>
+      <c r="B27" s="9" t="e">
         <f aca="false">HLOOKUP(A27,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B28" s="6" t="e">
+        <v>375</v>
+      </c>
+      <c r="B28" s="9" t="e">
         <f aca="false">HLOOKUP(A28,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B29" s="6" t="e">
+        <v>376</v>
+      </c>
+      <c r="B29" s="9" t="e">
         <f aca="false">HLOOKUP(A29,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B30" s="6" t="e">
+        <v>377</v>
+      </c>
+      <c r="B30" s="9" t="e">
         <f aca="false">HLOOKUP(A30,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" s="6" t="e">
+        <v>378</v>
+      </c>
+      <c r="B31" s="9" t="e">
         <f aca="false">HLOOKUP(A31,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="6" t="e">
+        <v>379</v>
+      </c>
+      <c r="B32" s="9" t="e">
         <f aca="false">HLOOKUP(A32,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="B33" s="6" t="e">
+        <v>380</v>
+      </c>
+      <c r="B33" s="9" t="e">
         <f aca="false">HLOOKUP(A33,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B34" s="6" t="e">
+        <v>381</v>
+      </c>
+      <c r="B34" s="9" t="e">
         <f aca="false">HLOOKUP(A34,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B35" s="6" t="e">
+        <v>382</v>
+      </c>
+      <c r="B35" s="9" t="e">
         <f aca="false">HLOOKUP(A35,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="B36" s="6" t="e">
+        <v>383</v>
+      </c>
+      <c r="B36" s="9" t="e">
         <f aca="false">HLOOKUP(A36,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B37" s="6" t="e">
+        <v>384</v>
+      </c>
+      <c r="B37" s="9" t="e">
         <f aca="false">HLOOKUP(A37,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B38" s="6" t="e">
+        <v>385</v>
+      </c>
+      <c r="B38" s="9" t="e">
         <f aca="false">HLOOKUP(A38,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" s="6" t="e">
+        <v>386</v>
+      </c>
+      <c r="B39" s="9" t="e">
         <f aca="false">HLOOKUP(A39,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" s="6" t="e">
+        <v>387</v>
+      </c>
+      <c r="B40" s="9" t="e">
         <f aca="false">HLOOKUP(A40,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="6" t="e">
+        <v>388</v>
+      </c>
+      <c r="B41" s="9" t="e">
         <f aca="false">HLOOKUP(A41,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B42" s="6" t="e">
+        <v>389</v>
+      </c>
+      <c r="B42" s="9" t="e">
         <f aca="false">HLOOKUP(A42,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B43" s="6" t="e">
+        <v>390</v>
+      </c>
+      <c r="B43" s="9" t="e">
         <f aca="false">HLOOKUP(A43,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B44" s="6" t="e">
+        <v>391</v>
+      </c>
+      <c r="B44" s="9" t="e">
         <f aca="false">HLOOKUP(A44,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B45" s="6" t="e">
+        <v>392</v>
+      </c>
+      <c r="B45" s="9" t="e">
         <f aca="false">HLOOKUP(A45,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B46" s="6" t="e">
+        <v>393</v>
+      </c>
+      <c r="B46" s="9" t="e">
         <f aca="false">HLOOKUP(A46,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B47" s="6" t="e">
+        <v>394</v>
+      </c>
+      <c r="B47" s="9" t="e">
         <f aca="false">HLOOKUP(A47,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="B48" s="6" t="e">
+        <v>395</v>
+      </c>
+      <c r="B48" s="9" t="e">
         <f aca="false">HLOOKUP(A48,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B49" s="6" t="e">
+        <v>396</v>
+      </c>
+      <c r="B49" s="9" t="e">
         <f aca="false">HLOOKUP(A49,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="B50" s="6" t="e">
+        <v>397</v>
+      </c>
+      <c r="B50" s="9" t="e">
         <f aca="false">HLOOKUP(A50,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B51" s="6" t="e">
+        <v>398</v>
+      </c>
+      <c r="B51" s="9" t="e">
         <f aca="false">HLOOKUP(A51,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B52" s="6" t="e">
+        <v>399</v>
+      </c>
+      <c r="B52" s="9" t="e">
         <f aca="false">HLOOKUP(A52,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="B53" s="6" t="e">
+        <v>400</v>
+      </c>
+      <c r="B53" s="9" t="e">
         <f aca="false">HLOOKUP(A53,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B54" s="6" t="e">
+        <v>401</v>
+      </c>
+      <c r="B54" s="9" t="e">
         <f aca="false">HLOOKUP(A54,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="B55" s="6" t="e">
+        <v>402</v>
+      </c>
+      <c r="B55" s="9" t="e">
         <f aca="false">HLOOKUP(A55,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="B56" s="6" t="e">
+        <v>403</v>
+      </c>
+      <c r="B56" s="9" t="e">
         <f aca="false">HLOOKUP(A56,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="B57" s="6" t="e">
+        <v>404</v>
+      </c>
+      <c r="B57" s="9" t="e">
         <f aca="false">HLOOKUP(A57,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B58" s="6" t="e">
+        <v>405</v>
+      </c>
+      <c r="B58" s="9" t="e">
         <f aca="false">HLOOKUP(A58,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="B59" s="6" t="e">
+        <v>406</v>
+      </c>
+      <c r="B59" s="9" t="e">
         <f aca="false">HLOOKUP(A59,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="B60" s="6" t="e">
+        <v>407</v>
+      </c>
+      <c r="B60" s="9" t="e">
         <f aca="false">HLOOKUP(A60,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="B61" s="6" t="e">
+        <v>408</v>
+      </c>
+      <c r="B61" s="9" t="e">
         <f aca="false">HLOOKUP(A61,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B62" s="6" t="e">
+        <v>409</v>
+      </c>
+      <c r="B62" s="9" t="e">
         <f aca="false">HLOOKUP(A62,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B63" s="6" t="e">
+        <v>410</v>
+      </c>
+      <c r="B63" s="9" t="e">
         <f aca="false">HLOOKUP(A63,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B64" s="6" t="e">
+        <v>411</v>
+      </c>
+      <c r="B64" s="9" t="e">
         <f aca="false">HLOOKUP(A64,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="B65" s="6" t="e">
+        <v>412</v>
+      </c>
+      <c r="B65" s="9" t="e">
         <f aca="false">HLOOKUP(A65,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B66" s="6" t="e">
+        <v>413</v>
+      </c>
+      <c r="B66" s="9" t="e">
         <f aca="false">HLOOKUP(A66,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B67" s="6" t="e">
+        <v>414</v>
+      </c>
+      <c r="B67" s="9" t="e">
         <f aca="false">HLOOKUP(A67,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B68" s="6" t="e">
+        <v>415</v>
+      </c>
+      <c r="B68" s="9" t="e">
         <f aca="false">HLOOKUP(A68,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B69" s="6" t="e">
+        <v>416</v>
+      </c>
+      <c r="B69" s="9" t="e">
         <f aca="false">HLOOKUP(A69,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="B70" s="6" t="e">
+        <v>417</v>
+      </c>
+      <c r="B70" s="9" t="e">
         <f aca="false">HLOOKUP(A70,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B71" s="6" t="e">
+        <v>418</v>
+      </c>
+      <c r="B71" s="9" t="e">
         <f aca="false">HLOOKUP(A71,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B72" s="6" t="e">
+        <v>419</v>
+      </c>
+      <c r="B72" s="9" t="e">
         <f aca="false">HLOOKUP(A72,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B73" s="6" t="e">
+        <v>420</v>
+      </c>
+      <c r="B73" s="9" t="e">
         <f aca="false">HLOOKUP(A73,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B74" s="6" t="e">
+        <v>421</v>
+      </c>
+      <c r="B74" s="9" t="e">
         <f aca="false">HLOOKUP(A74,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" s="6" t="e">
+        <v>422</v>
+      </c>
+      <c r="B75" s="9" t="e">
         <f aca="false">HLOOKUP(A75,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B76" s="6" t="e">
+        <v>423</v>
+      </c>
+      <c r="B76" s="9" t="e">
         <f aca="false">HLOOKUP(A76,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B77" s="6" t="e">
+        <v>424</v>
+      </c>
+      <c r="B77" s="9" t="e">
         <f aca="false">HLOOKUP(A77,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B78" s="6" t="e">
+        <v>425</v>
+      </c>
+      <c r="B78" s="9" t="e">
         <f aca="false">HLOOKUP(A78,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="B79" s="6" t="e">
+        <v>426</v>
+      </c>
+      <c r="B79" s="9" t="e">
         <f aca="false">HLOOKUP(A79,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="B80" s="6" t="e">
+        <v>427</v>
+      </c>
+      <c r="B80" s="9" t="e">
         <f aca="false">HLOOKUP(A80,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B81" s="6" t="e">
+        <v>428</v>
+      </c>
+      <c r="B81" s="9" t="e">
         <f aca="false">HLOOKUP(A81,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="B82" s="6" t="e">
+        <v>429</v>
+      </c>
+      <c r="B82" s="9" t="e">
         <f aca="false">HLOOKUP(A82,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="B83" s="6" t="e">
+        <v>430</v>
+      </c>
+      <c r="B83" s="9" t="e">
         <f aca="false">HLOOKUP(A83,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="B84" s="6" t="e">
+        <v>431</v>
+      </c>
+      <c r="B84" s="9" t="e">
         <f aca="false">HLOOKUP(A84,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="B85" s="6" t="e">
+        <v>432</v>
+      </c>
+      <c r="B85" s="9" t="e">
         <f aca="false">HLOOKUP(A85,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B86" s="6" t="e">
+        <v>433</v>
+      </c>
+      <c r="B86" s="9" t="e">
         <f aca="false">HLOOKUP(A86,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="B87" s="6" t="e">
+        <v>434</v>
+      </c>
+      <c r="B87" s="9" t="e">
         <f aca="false">HLOOKUP(A87,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="B88" s="6" t="e">
+        <v>435</v>
+      </c>
+      <c r="B88" s="9" t="e">
         <f aca="false">HLOOKUP(A88,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B89" s="6" t="e">
+        <v>436</v>
+      </c>
+      <c r="B89" s="9" t="e">
         <f aca="false">HLOOKUP(A89,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="B90" s="6" t="e">
+        <v>437</v>
+      </c>
+      <c r="B90" s="9" t="e">
         <f aca="false">HLOOKUP(A90,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="B91" s="6" t="e">
+        <v>438</v>
+      </c>
+      <c r="B91" s="9" t="e">
         <f aca="false">HLOOKUP(A91,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B92" s="6" t="e">
+        <v>439</v>
+      </c>
+      <c r="B92" s="9" t="e">
         <f aca="false">HLOOKUP(A92,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="B93" s="6" t="e">
+        <v>440</v>
+      </c>
+      <c r="B93" s="9" t="e">
         <f aca="false">HLOOKUP(A93,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B94" s="6" t="e">
+        <v>441</v>
+      </c>
+      <c r="B94" s="9" t="e">
         <f aca="false">HLOOKUP(A94,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="B95" s="6" t="e">
+        <v>442</v>
+      </c>
+      <c r="B95" s="9" t="e">
         <f aca="false">HLOOKUP(A95,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B96" s="6" t="e">
+        <v>443</v>
+      </c>
+      <c r="B96" s="9" t="e">
         <f aca="false">HLOOKUP(A96,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="B97" s="6" t="e">
+        <v>444</v>
+      </c>
+      <c r="B97" s="9" t="e">
         <f aca="false">HLOOKUP(A97,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B98" s="6" t="e">
+        <v>445</v>
+      </c>
+      <c r="B98" s="9" t="e">
         <f aca="false">HLOOKUP(A98,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="B99" s="6" t="e">
+        <v>446</v>
+      </c>
+      <c r="B99" s="9" t="e">
         <f aca="false">HLOOKUP(A99,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B100" s="6" t="e">
+        <v>447</v>
+      </c>
+      <c r="B100" s="9" t="e">
         <f aca="false">HLOOKUP(A100,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B101" s="6" t="e">
+        <v>448</v>
+      </c>
+      <c r="B101" s="9" t="e">
         <f aca="false">HLOOKUP(A101,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B102" s="6" t="e">
+        <v>211</v>
+      </c>
+      <c r="B102" s="9" t="e">
         <f aca="false">HLOOKUP(A102,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B103" s="6" t="e">
+        <v>449</v>
+      </c>
+      <c r="B103" s="9" t="e">
         <f aca="false">HLOOKUP(A103,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="B104" s="6" t="e">
+        <v>450</v>
+      </c>
+      <c r="B104" s="9" t="e">
         <f aca="false">HLOOKUP(A104,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B105" s="6" t="e">
+        <v>451</v>
+      </c>
+      <c r="B105" s="9" t="e">
         <f aca="false">HLOOKUP(A105,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B106" s="6" t="e">
+        <v>452</v>
+      </c>
+      <c r="B106" s="9" t="e">
         <f aca="false">HLOOKUP(A106,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="B107" s="6" t="e">
+        <v>453</v>
+      </c>
+      <c r="B107" s="9" t="e">
         <f aca="false">HLOOKUP(A107,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="B108" s="6" t="e">
+        <v>454</v>
+      </c>
+      <c r="B108" s="9" t="e">
         <f aca="false">HLOOKUP(A108,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="B109" s="6" t="e">
+        <v>455</v>
+      </c>
+      <c r="B109" s="9" t="e">
         <f aca="false">HLOOKUP(A109,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B110" s="6" t="e">
+        <v>456</v>
+      </c>
+      <c r="B110" s="9" t="e">
         <f aca="false">HLOOKUP(A110,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B111" s="6" t="e">
+        <v>457</v>
+      </c>
+      <c r="B111" s="9" t="e">
         <f aca="false">HLOOKUP(A111,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B112" s="6" t="e">
+        <v>458</v>
+      </c>
+      <c r="B112" s="9" t="e">
         <f aca="false">HLOOKUP(A112,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B113" s="6" t="e">
+        <v>459</v>
+      </c>
+      <c r="B113" s="9" t="e">
         <f aca="false">HLOOKUP(A113,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B114" s="6" t="e">
+        <v>460</v>
+      </c>
+      <c r="B114" s="9" t="e">
         <f aca="false">HLOOKUP(A114,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B115" s="6" t="e">
+        <v>461</v>
+      </c>
+      <c r="B115" s="9" t="e">
         <f aca="false">HLOOKUP(A115,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B116" s="6" t="e">
+        <v>462</v>
+      </c>
+      <c r="B116" s="9" t="e">
         <f aca="false">HLOOKUP(A116,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="B117" s="6" t="e">
+        <v>463</v>
+      </c>
+      <c r="B117" s="9" t="e">
         <f aca="false">HLOOKUP(A117,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B118" s="6" t="e">
+        <v>464</v>
+      </c>
+      <c r="B118" s="9" t="e">
         <f aca="false">HLOOKUP(A118,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B119" s="6" t="e">
+        <v>465</v>
+      </c>
+      <c r="B119" s="9" t="e">
         <f aca="false">HLOOKUP(A119,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="B120" s="6" t="e">
+        <v>466</v>
+      </c>
+      <c r="B120" s="9" t="e">
         <f aca="false">HLOOKUP(A120,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="B121" s="6" t="e">
+        <v>467</v>
+      </c>
+      <c r="B121" s="9" t="e">
         <f aca="false">HLOOKUP(A121,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="B122" s="6" t="e">
+        <v>468</v>
+      </c>
+      <c r="B122" s="9" t="e">
         <f aca="false">HLOOKUP(A122,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="B123" s="6" t="e">
+        <v>469</v>
+      </c>
+      <c r="B123" s="9" t="e">
         <f aca="false">HLOOKUP(A123,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="B124" s="6" t="e">
+        <v>470</v>
+      </c>
+      <c r="B124" s="9" t="e">
         <f aca="false">HLOOKUP(A124,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="B125" s="6" t="e">
+        <v>471</v>
+      </c>
+      <c r="B125" s="9" t="e">
         <f aca="false">HLOOKUP(A125,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B126" s="6" t="e">
+        <v>472</v>
+      </c>
+      <c r="B126" s="9" t="e">
         <f aca="false">HLOOKUP(A126,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B127" s="6" t="e">
+        <v>243</v>
+      </c>
+      <c r="B127" s="9" t="e">
         <f aca="false">HLOOKUP(A127,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B128" s="6" t="e">
+        <v>473</v>
+      </c>
+      <c r="B128" s="9" t="e">
         <f aca="false">HLOOKUP(A128,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B129" s="6" t="e">
+        <v>257</v>
+      </c>
+      <c r="B129" s="9" t="e">
         <f aca="false">HLOOKUP(A129,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B130" s="6" t="e">
+        <v>263</v>
+      </c>
+      <c r="B130" s="9" t="str">
         <f aca="false">HLOOKUP(A130,Munkalap1!H:I,2)</f>
-        <v>#N/A</v>
+        <v>http://bit.ly/334pYHg
+http://bit.ly/2Qz734H
+http://bit.ly/2O2CT8l</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="B131" s="6" t="e">
+        <v>474</v>
+      </c>
+      <c r="B131" s="9" t="e">
         <f aca="false">HLOOKUP(A131,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B132" s="6" t="e">
+        <v>475</v>
+      </c>
+      <c r="B132" s="9" t="e">
         <f aca="false">HLOOKUP(A132,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="B133" s="6" t="e">
+        <v>476</v>
+      </c>
+      <c r="B133" s="9" t="e">
         <f aca="false">HLOOKUP(A133,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="B134" s="6" t="e">
+        <v>477</v>
+      </c>
+      <c r="B134" s="9" t="e">
         <f aca="false">HLOOKUP(A134,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B135" s="6" t="e">
+        <v>278</v>
+      </c>
+      <c r="B135" s="9" t="str">
         <f aca="false">HLOOKUP(A135,Munkalap1!H:I,2)</f>
-        <v>#N/A</v>
+        <v>http://bit.ly/334pYHg
+http://bit.ly/2Qz734H
+http://bit.ly/2O2CT8l</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B136" s="6" t="e">
+        <v>284</v>
+      </c>
+      <c r="B136" s="9" t="e">
         <f aca="false">HLOOKUP(A136,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B137" s="6" t="e">
+        <v>290</v>
+      </c>
+      <c r="B137" s="9" t="str">
         <f aca="false">HLOOKUP(A137,Munkalap1!H:I,2)</f>
-        <v>#N/A</v>
+        <v>http://bit.ly/334pYHg
+http://bit.ly/2Qz734H
+http://bit.ly/2O2CT8l</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="B138" s="6" t="e">
+        <v>478</v>
+      </c>
+      <c r="B138" s="9" t="e">
         <f aca="false">HLOOKUP(A138,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B139" s="6" t="e">
+        <v>479</v>
+      </c>
+      <c r="B139" s="9" t="e">
         <f aca="false">HLOOKUP(A139,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="B140" s="6" t="e">
+        <v>480</v>
+      </c>
+      <c r="B140" s="9" t="e">
         <f aca="false">HLOOKUP(A140,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="B141" s="6" t="e">
+        <v>481</v>
+      </c>
+      <c r="B141" s="9" t="e">
         <f aca="false">HLOOKUP(A141,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B142" s="6" t="e">
+        <v>305</v>
+      </c>
+      <c r="B142" s="9" t="e">
         <f aca="false">HLOOKUP(A142,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="B143" s="6" t="e">
+        <v>482</v>
+      </c>
+      <c r="B143" s="9" t="e">
         <f aca="false">HLOOKUP(A143,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="B144" s="6" t="e">
+        <v>483</v>
+      </c>
+      <c r="B144" s="9" t="e">
         <f aca="false">HLOOKUP(A144,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B145" s="6" t="e">
+        <v>484</v>
+      </c>
+      <c r="B145" s="9" t="e">
         <f aca="false">HLOOKUP(A145,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="B146" s="6" t="e">
+        <v>485</v>
+      </c>
+      <c r="B146" s="9" t="e">
         <f aca="false">HLOOKUP(A146,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="B147" s="6" t="e">
+        <v>486</v>
+      </c>
+      <c r="B147" s="9" t="e">
         <f aca="false">HLOOKUP(A147,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B148" s="6" t="e">
+        <v>320</v>
+      </c>
+      <c r="B148" s="9" t="str">
         <f aca="false">HLOOKUP(A148,Munkalap1!H:I,2)</f>
-        <v>#N/A</v>
+        <v>http://bit.ly/334pYHg
+http://bit.ly/2Qz734H
+http://bit.ly/2O2CT8l</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B149" s="6" t="e">
+        <v>326</v>
+      </c>
+      <c r="B149" s="9" t="str">
         <f aca="false">HLOOKUP(A149,Munkalap1!H:I,2)</f>
-        <v>#N/A</v>
+        <v>http://bit.ly/334pYHg
+http://bit.ly/2Qz734H
+http://bit.ly/2O2CT8l</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B150" s="6" t="e">
+        <v>487</v>
+      </c>
+      <c r="B150" s="9" t="e">
         <f aca="false">HLOOKUP(A150,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B151" s="6" t="e">
+        <v>488</v>
+      </c>
+      <c r="B151" s="9" t="e">
         <f aca="false">HLOOKUP(A151,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="B152" s="6" t="e">
+        <v>489</v>
+      </c>
+      <c r="B152" s="9" t="e">
         <f aca="false">HLOOKUP(A152,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="B153" s="6" t="e">
+        <v>490</v>
+      </c>
+      <c r="B153" s="9" t="e">
         <f aca="false">HLOOKUP(A153,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B154" s="6" t="e">
+        <v>491</v>
+      </c>
+      <c r="B154" s="9" t="e">
         <f aca="false">HLOOKUP(A154,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="B155" s="6" t="e">
+        <v>492</v>
+      </c>
+      <c r="B155" s="9" t="e">
         <f aca="false">HLOOKUP(A155,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B156" s="6" t="e">
+        <v>342</v>
+      </c>
+      <c r="B156" s="9" t="e">
         <f aca="false">HLOOKUP(A156,Munkalap1!H:I,2)</f>
         <v>#N/A</v>
       </c>

</xml_diff>